<commit_message>
Add events hub and the code for the table
</commit_message>
<xml_diff>
--- a/ProjectInfo.xlsx
+++ b/ProjectInfo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
   <si>
     <t>Client</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>On talbe</t>
+  </si>
+  <si>
+    <t>after end date</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <dimension ref="B1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C5" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +853,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -865,7 +868,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -879,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -893,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -910,12 +913,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -929,7 +932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>64</v>
       </c>
@@ -943,7 +946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -957,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>65</v>
       </c>
@@ -974,7 +977,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>67</v>
       </c>
@@ -991,7 +994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>47</v>
       </c>
@@ -1000,7 +1003,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -1016,8 +1019,11 @@
       <c r="F28" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>39</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>43</v>
       </c>
@@ -1050,8 +1056,11 @@
       <c r="F30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>46</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>48</v>
       </c>

</xml_diff>